<commit_message>
Innlesing av sluttspill støttet
</commit_message>
<xml_diff>
--- a/PredictionSheets/VM 2014 Tippekonkuranse_AndreasF.xlsx
+++ b/PredictionSheets/VM 2014 Tippekonkuranse_AndreasF.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\226568\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9576" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="9570"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppespilltipp" sheetId="1" r:id="rId1"/>
     <sheet name="Sluttspilltipp" sheetId="2" r:id="rId2"/>
     <sheet name="Kampoppsett" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="139">
   <si>
     <t>Group A</t>
   </si>
@@ -440,17 +435,20 @@
   </si>
   <si>
     <t>Korea</t>
+  </si>
+  <si>
+    <t>Andreas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-414]d/\ mmmm;@"/>
     <numFmt numFmtId="165" formatCode="hh:mm;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1784,23 +1782,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="11" width="14.44140625" customWidth="1"/>
+    <col min="1" max="11" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="21">
       <c r="B1" s="19" t="s">
         <v>44</v>
       </c>
@@ -1810,17 +1808,19 @@
       <c r="N1" s="64"/>
       <c r="O1" s="64"/>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1">
       <c r="L2" s="64"/>
       <c r="M2" s="64"/>
       <c r="N2" s="64"/>
       <c r="O2" s="64"/>
     </row>
-    <row r="3" spans="1:15" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="28.15" customHeight="1" thickBot="1">
       <c r="A3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="16"/>
+      <c r="B3" s="16" t="s">
+        <v>138</v>
+      </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="18"/>
@@ -1829,13 +1829,13 @@
       <c r="N3" s="64"/>
       <c r="O3" s="64"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15">
       <c r="L4" s="64"/>
       <c r="M4" s="64"/>
       <c r="N4" s="64"/>
       <c r="O4" s="64"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15">
       <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="15.75" thickBot="1">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="28.15" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>1</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="28.15" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>3</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="28.15" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>1</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="28.15" customHeight="1">
       <c r="A14" s="8" t="s">
         <v>4</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="28.15" customHeight="1">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="28.15" customHeight="1" thickBot="1">
       <c r="A16" s="10" t="s">
         <v>2</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="20.25" customHeight="1">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
@@ -2106,7 +2106,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="20.25" customHeight="1" thickBot="1">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -2120,7 +2120,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="28.15" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>6</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="28.15" customHeight="1">
       <c r="A20" s="8" t="s">
         <v>8</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="28.15" customHeight="1">
       <c r="A21" s="8" t="s">
         <v>6</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="28.15" customHeight="1">
       <c r="A22" s="8" t="s">
         <v>9</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="28.15" customHeight="1">
       <c r="A23" s="8" t="s">
         <v>9</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="28.15" customHeight="1" thickBot="1">
       <c r="A24" s="10" t="s">
         <v>7</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="20.25" customHeight="1">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
@@ -2332,7 +2332,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="20.25" customHeight="1" thickBot="1">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2346,7 +2346,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="28.15" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>11</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="28.15" customHeight="1">
       <c r="A28" s="8" t="s">
         <v>13</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="28.15" customHeight="1">
       <c r="A29" s="8" t="s">
         <v>11</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="28.15" customHeight="1">
       <c r="A30" s="8" t="s">
         <v>14</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="28.15" customHeight="1">
       <c r="A31" s="8" t="s">
         <v>14</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="28.15" customHeight="1" thickBot="1">
       <c r="A32" s="10" t="s">
         <v>12</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="20.25" customHeight="1">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="2"/>
@@ -2558,7 +2558,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="20.25" customHeight="1" thickBot="1">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -2572,7 +2572,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="28.15" customHeight="1">
       <c r="A35" s="6" t="s">
         <v>16</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="28.15" customHeight="1">
       <c r="A36" s="8" t="s">
         <v>18</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="28.15" customHeight="1">
       <c r="A37" s="8" t="s">
         <v>16</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="28.15" customHeight="1">
       <c r="A38" s="8" t="s">
         <v>19</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="28.15" customHeight="1">
       <c r="A39" s="8" t="s">
         <v>19</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="28.15" customHeight="1" thickBot="1">
       <c r="A40" s="10" t="s">
         <v>17</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11">
       <c r="A42" s="21"/>
     </row>
   </sheetData>
@@ -2792,35 +2792,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1">
       <c r="A3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="24" customHeight="1">
       <c r="A4" s="22" t="s">
         <v>130</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="24" customHeight="1">
       <c r="A5" s="25" t="s">
         <v>131</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="24" customHeight="1">
       <c r="A6" s="25" t="s">
         <v>132</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="24" customHeight="1" thickBot="1">
       <c r="A7" s="28" t="s">
         <v>8</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1">
       <c r="A10" s="31" t="s">
         <v>47</v>
       </c>
@@ -2884,7 +2884,7 @@
       <c r="C10" s="32"/>
       <c r="D10" s="32"/>
     </row>
-    <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="24" customHeight="1">
       <c r="A11" s="33" t="s">
         <v>130</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="24" customHeight="1" thickBot="1">
       <c r="A12" s="36" t="s">
         <v>133</v>
       </c>
@@ -2912,12 +2912,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1">
       <c r="A15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="24" customHeight="1" thickBot="1">
       <c r="A16" s="39" t="s">
         <v>135</v>
       </c>
@@ -2931,12 +2931,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1">
       <c r="A19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1">
       <c r="A20" s="42" t="s">
         <v>130</v>
       </c>
@@ -2962,7 +2962,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
@@ -2973,15 +2973,15 @@
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="47"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="47"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="50">
         <v>41802</v>
       </c>
@@ -3007,7 +3007,7 @@
       </c>
       <c r="G2" s="48"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="54">
         <v>41803</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="54">
         <v>41807</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="54">
         <v>41809</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" s="54">
         <v>41813</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" s="57">
         <v>41813</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" s="61"/>
       <c r="B8" s="62"/>
       <c r="C8" s="21"/>
@@ -3161,7 +3161,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9" s="50">
         <v>41803</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11">
       <c r="A10" s="54">
         <v>41804</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="A11" s="54">
         <v>41808</v>
       </c>
@@ -3231,7 +3231,7 @@
       <c r="F11" s="46"/>
       <c r="G11" s="49"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="A12" s="54">
         <v>41808</v>
       </c>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="G12" s="49"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11">
       <c r="A13" s="54">
         <v>41813</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11">
       <c r="A14" s="57">
         <v>41813</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="64" customFormat="1">
       <c r="A15" s="61"/>
       <c r="B15" s="62"/>
       <c r="C15" s="21"/>
@@ -3322,7 +3322,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11">
       <c r="A16" s="50">
         <v>41804</v>
       </c>
@@ -3351,7 +3351,7 @@
       </c>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10">
       <c r="A17" s="54">
         <v>41805</v>
       </c>
@@ -3367,7 +3367,7 @@
       <c r="F17" s="46"/>
       <c r="G17" s="49"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18" s="54">
         <v>41809</v>
       </c>
@@ -3385,7 +3385,7 @@
       </c>
       <c r="G18" s="49"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="A19" s="54">
         <v>41810</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="A20" s="54">
         <v>41814</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="A21" s="57">
         <v>41814</v>
       </c>
@@ -3455,7 +3455,7 @@
       <c r="F21" s="46"/>
       <c r="G21" s="49"/>
     </row>
-    <row r="22" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" s="64" customFormat="1">
       <c r="A22" s="61"/>
       <c r="B22" s="62"/>
       <c r="C22" s="21"/>
@@ -3465,7 +3465,7 @@
       </c>
       <c r="G22" s="66"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23" s="50">
         <v>41804</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24" s="54">
         <v>41805</v>
       </c>
@@ -3506,7 +3506,7 @@
       <c r="F24" s="46"/>
       <c r="G24" s="49"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10">
       <c r="A25" s="54">
         <v>41809</v>
       </c>
@@ -3524,7 +3524,7 @@
       </c>
       <c r="G25" s="49"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10">
       <c r="A26" s="54">
         <v>41810</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10">
       <c r="A27" s="54">
         <v>41814</v>
       </c>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="F27" s="45"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10">
       <c r="A28" s="57">
         <v>41814</v>
       </c>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="F28" s="45"/>
     </row>
-    <row r="29" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" s="64" customFormat="1">
       <c r="A29" s="61"/>
       <c r="B29" s="62"/>
       <c r="C29" s="21"/>
@@ -3587,7 +3587,7 @@
       <c r="F29" s="67"/>
       <c r="G29" s="68"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10">
       <c r="A30" s="50">
         <v>41805</v>
       </c>
@@ -3605,7 +3605,7 @@
       <c r="G30" s="86"/>
       <c r="H30" s="87"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10">
       <c r="A31" s="54">
         <v>41805</v>
       </c>
@@ -3620,7 +3620,7 @@
       </c>
       <c r="F31" s="45"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10">
       <c r="A32" s="54">
         <v>41810</v>
       </c>
@@ -3635,7 +3635,7 @@
       </c>
       <c r="F32" s="45"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33" s="54">
         <v>41811</v>
       </c>
@@ -3650,7 +3650,7 @@
       </c>
       <c r="F33" s="45"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7">
       <c r="A34" s="54">
         <v>41815</v>
       </c>
@@ -3665,7 +3665,7 @@
       </c>
       <c r="F34" s="45"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7">
       <c r="A35" s="57">
         <v>41815</v>
       </c>
@@ -3680,14 +3680,14 @@
       </c>
       <c r="F35" s="45"/>
     </row>
-    <row r="36" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" s="64" customFormat="1">
       <c r="A36" s="61"/>
       <c r="B36" s="62"/>
       <c r="C36" s="21"/>
       <c r="D36" s="63"/>
       <c r="G36" s="68"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7">
       <c r="A37" s="50">
         <v>41806</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7">
       <c r="A38" s="54">
         <v>41806</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7">
       <c r="A39" s="54">
         <v>41811</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7">
       <c r="A40" s="54">
         <v>41812</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7">
       <c r="A41" s="54">
         <v>41815</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7">
       <c r="A42" s="57">
         <v>41815</v>
       </c>
@@ -3771,14 +3771,14 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" s="64" customFormat="1">
       <c r="A43" s="61"/>
       <c r="B43" s="62"/>
       <c r="C43" s="21"/>
       <c r="D43" s="63"/>
       <c r="G43" s="68"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7">
       <c r="A44" s="50">
         <v>41806</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7">
       <c r="A45" s="54">
         <v>41807</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7">
       <c r="A46" s="54">
         <v>41811</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7">
       <c r="A47" s="54">
         <v>41813</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7">
       <c r="A48" s="54">
         <v>41816</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7">
       <c r="A49" s="57">
         <v>41816</v>
       </c>
@@ -3862,14 +3862,14 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" s="64" customFormat="1">
       <c r="A50" s="61"/>
       <c r="B50" s="62"/>
       <c r="C50" s="21"/>
       <c r="D50" s="63"/>
       <c r="G50" s="68"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7">
       <c r="A51" s="50">
         <v>41807</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7">
       <c r="A52" s="54">
         <v>41808</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7">
       <c r="A53" s="54">
         <v>41812</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7">
       <c r="A54" s="54">
         <v>41812</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7">
       <c r="A55" s="54">
         <v>41816</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7">
       <c r="A56" s="57">
         <v>41816</v>
       </c>

</xml_diff>